<commit_message>
Update before peeling off for separate RMd per cell type
</commit_message>
<xml_diff>
--- a/data/cluster-interpretation-nov23.xlsx
+++ b/data/cluster-interpretation-nov23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kierancampbell/toronto/cytomarker-paper-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6489054E-06F3-DF41-8DEC-A696A3D085A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA44A149-DF55-C64B-8EA9-736FF6121B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1780" yWindow="1780" windowWidth="27640" windowHeight="16940" xr2:uid="{BC73D4BA-6954-FE4C-BCD7-3400F4DE2537}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>cluster</t>
   </si>
@@ -47,9 +47,6 @@
     <t>T-CD8</t>
   </si>
   <si>
-    <t>T-CD4-CD16</t>
-  </si>
-  <si>
     <t>T-CD4</t>
   </si>
   <si>
@@ -60,6 +57,12 @@
   </si>
   <si>
     <t>Doublets</t>
+  </si>
+  <si>
+    <t>NK</t>
+  </si>
+  <si>
+    <t>Monocytes</t>
   </si>
 </sst>
 </file>
@@ -414,7 +417,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="152" zoomScaleNormal="152" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -431,11 +434,17 @@
       <c r="A2">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -458,7 +467,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -466,7 +475,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -474,7 +483,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -482,7 +491,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -490,7 +499,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>